<commit_message>
updated distributor in screaming circuits bom
</commit_message>
<xml_diff>
--- a/eagle/powerblade/powerblade_3v3_bom.xlsx
+++ b/eagle/powerblade/powerblade_3v3_bom.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="14385"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19180"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,12 @@
   <definedNames>
     <definedName name="powerblade_3v3_bom" localSheetId="0">Sheet1!$C$1:$J$61</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -680,9 +685,6 @@
     <t>UREACH_XTEND</t>
   </si>
   <si>
-    <t>FR05-S1-N-0-110</t>
-  </si>
-  <si>
     <t>C6, C34</t>
   </si>
   <si>
@@ -725,9 +727,6 @@
     <t>DigiKey</t>
   </si>
   <si>
-    <t>Fractus</t>
-  </si>
-  <si>
     <t>Dist Part #</t>
   </si>
   <si>
@@ -765,16 +764,38 @@
   </si>
   <si>
     <t>BGA per board</t>
+  </si>
+  <si>
+    <t>RichardsonRFPD</t>
+  </si>
+  <si>
+    <t>FR05-S1-N-0-110B</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -804,11 +825,11 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -816,17 +837,17 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -836,7 +857,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -844,45 +865,53 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1188,26 +1217,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="I62" sqref="I62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="5" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="5" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="61" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.28515625" customWidth="1"/>
-    <col min="9" max="9" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.33203125" customWidth="1"/>
+    <col min="9" max="9" width="22.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B1" t="s">
         <v>223</v>
-      </c>
-      <c r="B1" t="s">
-        <v>224</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1225,16 +1254,16 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="J1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1257,16 +1286,16 @@
         <v>7</v>
       </c>
       <c r="H2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
       </c>
       <c r="J2" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1289,16 +1318,16 @@
         <v>13</v>
       </c>
       <c r="H3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I3" t="s">
         <v>14</v>
       </c>
       <c r="J3" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1321,16 +1350,16 @@
         <v>19</v>
       </c>
       <c r="H4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I4" t="s">
         <v>39</v>
       </c>
       <c r="J4" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1338,7 +1367,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D5" t="s">
         <v>40</v>
@@ -1353,16 +1382,16 @@
         <v>43</v>
       </c>
       <c r="H5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I5" t="s">
         <v>44</v>
       </c>
       <c r="J5" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1385,16 +1414,16 @@
         <v>19</v>
       </c>
       <c r="H6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I6" t="s">
         <v>47</v>
       </c>
       <c r="J6" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1417,16 +1446,16 @@
         <v>19</v>
       </c>
       <c r="H7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I7" t="s">
         <v>50</v>
       </c>
       <c r="J7" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1449,16 +1478,16 @@
         <v>43</v>
       </c>
       <c r="H8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I8" t="s">
         <v>53</v>
       </c>
       <c r="J8" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1466,7 +1495,7 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D9" t="s">
         <v>54</v>
@@ -1481,16 +1510,16 @@
         <v>43</v>
       </c>
       <c r="H9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I9" t="s">
         <v>55</v>
       </c>
       <c r="J9" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1513,16 +1542,16 @@
         <v>19</v>
       </c>
       <c r="H10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I10" t="s">
         <v>20</v>
       </c>
       <c r="J10" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1545,16 +1574,16 @@
         <v>43</v>
       </c>
       <c r="H11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I11" t="s">
         <v>58</v>
       </c>
       <c r="J11" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1577,16 +1606,16 @@
         <v>43</v>
       </c>
       <c r="H12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I12" t="s">
         <v>61</v>
       </c>
       <c r="J12" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1609,16 +1638,16 @@
         <v>43</v>
       </c>
       <c r="H13" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I13" t="s">
         <v>64</v>
       </c>
       <c r="J13" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1626,7 +1655,7 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D14" t="s">
         <v>21</v>
@@ -1641,16 +1670,16 @@
         <v>19</v>
       </c>
       <c r="H14" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I14" t="s">
         <v>24</v>
       </c>
       <c r="J14" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1673,16 +1702,16 @@
         <v>19</v>
       </c>
       <c r="H15" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I15" t="s">
         <v>67</v>
       </c>
       <c r="J15" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1705,16 +1734,16 @@
         <v>19</v>
       </c>
       <c r="H16" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I16" t="s">
         <v>27</v>
       </c>
       <c r="J16" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1737,16 +1766,16 @@
         <v>19</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>29</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1754,7 +1783,7 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D18" t="s">
         <v>32</v>
@@ -1769,16 +1798,16 @@
         <v>19</v>
       </c>
       <c r="H18" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I18" t="s">
         <v>33</v>
       </c>
       <c r="J18" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1801,16 +1830,16 @@
         <v>19</v>
       </c>
       <c r="H19" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I19" t="s">
         <v>36</v>
       </c>
       <c r="J19" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1818,7 +1847,7 @@
         <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D20" t="s">
         <v>16</v>
@@ -1833,16 +1862,16 @@
         <v>19</v>
       </c>
       <c r="H20" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I20" t="s">
         <v>37</v>
       </c>
       <c r="J20" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1862,16 +1891,16 @@
         <v>70</v>
       </c>
       <c r="H21" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I21" t="s">
         <v>71</v>
       </c>
       <c r="J21" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1891,16 +1920,16 @@
         <v>74</v>
       </c>
       <c r="H22" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I22" t="s">
         <v>75</v>
       </c>
       <c r="J22" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1921,16 +1950,16 @@
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>29</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1951,16 +1980,16 @@
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>29</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1983,16 +2012,16 @@
         <v>86</v>
       </c>
       <c r="H25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I25" t="s">
         <v>87</v>
       </c>
       <c r="J25" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2012,16 +2041,16 @@
         <v>42</v>
       </c>
       <c r="H26" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I26" t="s">
         <v>91</v>
       </c>
       <c r="J26" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2041,16 +2070,16 @@
         <v>86</v>
       </c>
       <c r="H27" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I27" t="s">
         <v>93</v>
       </c>
       <c r="J27" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2073,16 +2102,16 @@
         <v>86</v>
       </c>
       <c r="H28" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I28" t="s">
         <v>96</v>
       </c>
       <c r="J28" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2102,16 +2131,16 @@
         <v>99</v>
       </c>
       <c r="H29" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I29" t="s">
         <v>100</v>
       </c>
       <c r="J29" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2131,16 +2160,16 @@
         <v>99</v>
       </c>
       <c r="H30" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I30" t="s">
         <v>103</v>
       </c>
       <c r="J30" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2148,7 +2177,7 @@
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D31" t="s">
         <v>133</v>
@@ -2163,16 +2192,16 @@
         <v>108</v>
       </c>
       <c r="H31" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I31" t="s">
         <v>134</v>
       </c>
       <c r="J31" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2195,16 +2224,16 @@
         <v>108</v>
       </c>
       <c r="H32" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I32" t="s">
         <v>136</v>
       </c>
       <c r="J32" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2212,7 +2241,7 @@
         <v>4</v>
       </c>
       <c r="C33" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D33" t="s">
         <v>137</v>
@@ -2227,16 +2256,16 @@
         <v>108</v>
       </c>
       <c r="H33" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I33" t="s">
         <v>138</v>
       </c>
       <c r="J33" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2259,16 +2288,16 @@
         <v>108</v>
       </c>
       <c r="H34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I34" t="s">
         <v>141</v>
       </c>
       <c r="J34" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2291,16 +2320,16 @@
         <v>108</v>
       </c>
       <c r="H35" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I35" t="s">
         <v>144</v>
       </c>
       <c r="J35" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2323,16 +2352,16 @@
         <v>108</v>
       </c>
       <c r="H36" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I36" t="s">
         <v>147</v>
       </c>
       <c r="J36" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2355,16 +2384,16 @@
         <v>108</v>
       </c>
       <c r="H37" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I37" t="s">
         <v>150</v>
       </c>
       <c r="J37" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2387,16 +2416,16 @@
         <v>108</v>
       </c>
       <c r="H38" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I38" t="s">
         <v>109</v>
       </c>
       <c r="J38" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2419,16 +2448,16 @@
         <v>108</v>
       </c>
       <c r="H39" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I39" t="s">
         <v>155</v>
       </c>
       <c r="J39" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2451,16 +2480,16 @@
         <v>108</v>
       </c>
       <c r="H40" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I40" t="s">
         <v>114</v>
       </c>
       <c r="J40" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2483,16 +2512,16 @@
         <v>108</v>
       </c>
       <c r="H41" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I41" t="s">
         <v>158</v>
       </c>
       <c r="J41" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2515,16 +2544,16 @@
         <v>108</v>
       </c>
       <c r="H42" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I42" t="s">
         <v>161</v>
       </c>
       <c r="J42" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2547,16 +2576,16 @@
         <v>108</v>
       </c>
       <c r="H43" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I43" t="s">
         <v>164</v>
       </c>
       <c r="J43" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2579,16 +2608,16 @@
         <v>108</v>
       </c>
       <c r="H44" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I44" t="s">
         <v>167</v>
       </c>
       <c r="J44" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2611,16 +2640,16 @@
         <v>119</v>
       </c>
       <c r="H45" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I45" t="s">
         <v>120</v>
       </c>
       <c r="J45" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2628,10 +2657,10 @@
         <v>3</v>
       </c>
       <c r="C46" t="s">
+        <v>219</v>
+      </c>
+      <c r="D46" t="s">
         <v>220</v>
-      </c>
-      <c r="D46" t="s">
-        <v>221</v>
       </c>
       <c r="E46" t="s">
         <v>121</v>
@@ -2643,16 +2672,16 @@
         <v>108</v>
       </c>
       <c r="H46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I46" t="s">
         <v>123</v>
       </c>
       <c r="J46" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2675,16 +2704,16 @@
         <v>108</v>
       </c>
       <c r="H47" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I47" t="s">
         <v>126</v>
       </c>
       <c r="J47" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2707,16 +2736,16 @@
         <v>108</v>
       </c>
       <c r="H48" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I48" t="s">
         <v>129</v>
       </c>
       <c r="J48" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2739,16 +2768,16 @@
         <v>108</v>
       </c>
       <c r="H49" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I49" t="s">
         <v>132</v>
       </c>
       <c r="J49" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2771,16 +2800,16 @@
         <v>108</v>
       </c>
       <c r="H50" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I50" t="s">
         <v>170</v>
       </c>
       <c r="J50" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2788,7 +2817,7 @@
         <v>2</v>
       </c>
       <c r="C51" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D51" t="s">
         <v>171</v>
@@ -2803,16 +2832,16 @@
         <v>108</v>
       </c>
       <c r="H51" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I51" t="s">
         <v>172</v>
       </c>
       <c r="J51" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -2833,16 +2862,16 @@
         <v>176</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I52" s="1" t="s">
         <v>177</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2862,16 +2891,16 @@
         <v>180</v>
       </c>
       <c r="H53" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I53" t="s">
         <v>181</v>
       </c>
       <c r="J53" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2882,25 +2911,25 @@
         <v>182</v>
       </c>
       <c r="D54" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E54" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F54" t="s">
         <v>183</v>
       </c>
       <c r="H54" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I54" t="s">
         <v>184</v>
       </c>
       <c r="J54" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2920,16 +2949,16 @@
         <v>187</v>
       </c>
       <c r="H55" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I55" t="s">
         <v>188</v>
       </c>
       <c r="J55" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2952,16 +2981,16 @@
         <v>192</v>
       </c>
       <c r="H56" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I56" t="s">
         <v>193</v>
       </c>
       <c r="J56" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2981,16 +3010,16 @@
         <v>183</v>
       </c>
       <c r="H57" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I57" t="s">
         <v>196</v>
       </c>
       <c r="J57" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
       <c r="A58">
         <v>57</v>
       </c>
@@ -3010,16 +3039,16 @@
         <v>199</v>
       </c>
       <c r="H58" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I58" t="s">
         <v>200</v>
       </c>
       <c r="J58" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
       <c r="A59">
         <v>58</v>
       </c>
@@ -3042,16 +3071,16 @@
         <v>204</v>
       </c>
       <c r="H59" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I59" t="s">
         <v>205</v>
       </c>
       <c r="J59" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
       <c r="A60">
         <v>59</v>
       </c>
@@ -3071,16 +3100,16 @@
         <v>805</v>
       </c>
       <c r="H60" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I60" t="s">
         <v>209</v>
       </c>
       <c r="J60" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
       <c r="A61">
         <v>60</v>
       </c>
@@ -3100,58 +3129,58 @@
         <v>211</v>
       </c>
       <c r="H61" t="s">
-        <v>227</v>
+        <v>239</v>
       </c>
       <c r="I61" t="s">
-        <v>212</v>
+        <v>240</v>
       </c>
       <c r="J61" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="65" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H65" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="65" spans="8:9">
+      <c r="H65" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="I65" s="7"/>
+    </row>
+    <row r="66" spans="8:9">
+      <c r="H66" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="I66" s="3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="67" spans="8:9">
+      <c r="H67" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="I65" s="3"/>
-    </row>
-    <row r="66" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H66" s="4" t="s">
+      <c r="I67" s="3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="68" spans="8:9">
+      <c r="H68" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="I68" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="8:9">
+      <c r="H69" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="I66" s="5">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="67" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H67" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="I67" s="5">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="68" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H68" s="4" t="s">
+      <c r="I69" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="8:9">
+      <c r="H70" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="I68" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H69" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="I69" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="70" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H70" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="I70" s="7">
+      <c r="I70" s="5">
         <v>1</v>
       </c>
     </row>
@@ -3163,6 +3192,12 @@
     <mergeCell ref="H65:I65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3172,9 +3207,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3184,8 +3224,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated version number in boards and changed a part number in excel
</commit_message>
<xml_diff>
--- a/eagle/powerblade/powerblade_3v3_bom.xlsx
+++ b/eagle/powerblade/powerblade_3v3_bom.xlsx
@@ -121,9 +121,6 @@
     <t>C0603_SM</t>
   </si>
   <si>
-    <t>445-9077-1-ND</t>
-  </si>
-  <si>
     <t>C4</t>
   </si>
   <si>
@@ -770,6 +767,9 @@
   </si>
   <si>
     <t>FR05-S1-N-0-110B</t>
+  </si>
+  <si>
+    <t>1276-1274-1-ND</t>
   </si>
 </sst>
 </file>
@@ -1217,8 +1217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="I62" sqref="I62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1233,10 +1233,10 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B1" t="s">
         <v>222</v>
-      </c>
-      <c r="B1" t="s">
-        <v>223</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1254,13 +1254,13 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I1" t="s">
+        <v>225</v>
+      </c>
+      <c r="J1" t="s">
         <v>226</v>
-      </c>
-      <c r="J1" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -1286,13 +1286,13 @@
         <v>7</v>
       </c>
       <c r="H2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
       </c>
       <c r="J2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1318,13 +1318,13 @@
         <v>13</v>
       </c>
       <c r="H3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I3" t="s">
         <v>14</v>
       </c>
       <c r="J3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1335,10 +1335,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
         <v>17</v>
@@ -1350,13 +1350,13 @@
         <v>19</v>
       </c>
       <c r="H4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -1367,28 +1367,28 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" t="s">
         <v>40</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>41</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>42</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
+        <v>224</v>
+      </c>
+      <c r="I5" t="s">
         <v>43</v>
       </c>
-      <c r="H5" t="s">
-        <v>225</v>
-      </c>
-      <c r="I5" t="s">
-        <v>44</v>
-      </c>
       <c r="J5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1399,10 +1399,10 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" t="s">
         <v>45</v>
-      </c>
-      <c r="D6" t="s">
-        <v>46</v>
       </c>
       <c r="E6" t="s">
         <v>22</v>
@@ -1414,13 +1414,13 @@
         <v>19</v>
       </c>
       <c r="H6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1431,10 +1431,10 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" t="s">
         <v>48</v>
-      </c>
-      <c r="D7" t="s">
-        <v>49</v>
       </c>
       <c r="E7" t="s">
         <v>17</v>
@@ -1446,13 +1446,13 @@
         <v>19</v>
       </c>
       <c r="H7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1463,28 +1463,28 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" t="s">
         <v>51</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" t="s">
+        <v>224</v>
+      </c>
+      <c r="I8" t="s">
         <v>52</v>
       </c>
-      <c r="E8" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G8" t="s">
-        <v>43</v>
-      </c>
-      <c r="H8" t="s">
-        <v>225</v>
-      </c>
-      <c r="I8" t="s">
-        <v>53</v>
-      </c>
       <c r="J8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1495,28 +1495,28 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" t="s">
+        <v>224</v>
+      </c>
+      <c r="I9" t="s">
         <v>54</v>
       </c>
-      <c r="E9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" t="s">
-        <v>43</v>
-      </c>
-      <c r="H9" t="s">
-        <v>225</v>
-      </c>
-      <c r="I9" t="s">
-        <v>55</v>
-      </c>
       <c r="J9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1542,13 +1542,13 @@
         <v>19</v>
       </c>
       <c r="H10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I10" t="s">
         <v>20</v>
       </c>
       <c r="J10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1559,28 +1559,28 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" t="s">
         <v>56</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" t="s">
+        <v>224</v>
+      </c>
+      <c r="I11" t="s">
         <v>57</v>
       </c>
-      <c r="E11" t="s">
-        <v>41</v>
-      </c>
-      <c r="F11" t="s">
-        <v>42</v>
-      </c>
-      <c r="G11" t="s">
-        <v>43</v>
-      </c>
-      <c r="H11" t="s">
-        <v>225</v>
-      </c>
-      <c r="I11" t="s">
-        <v>58</v>
-      </c>
       <c r="J11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1591,28 +1591,28 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" t="s">
         <v>59</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" t="s">
+        <v>42</v>
+      </c>
+      <c r="H12" t="s">
+        <v>224</v>
+      </c>
+      <c r="I12" t="s">
         <v>60</v>
       </c>
-      <c r="E12" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" t="s">
-        <v>42</v>
-      </c>
-      <c r="G12" t="s">
-        <v>43</v>
-      </c>
-      <c r="H12" t="s">
-        <v>225</v>
-      </c>
-      <c r="I12" t="s">
-        <v>61</v>
-      </c>
       <c r="J12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1623,28 +1623,28 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" t="s">
         <v>62</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13" t="s">
+        <v>224</v>
+      </c>
+      <c r="I13" t="s">
         <v>63</v>
       </c>
-      <c r="E13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F13" t="s">
-        <v>42</v>
-      </c>
-      <c r="G13" t="s">
-        <v>43</v>
-      </c>
-      <c r="H13" t="s">
-        <v>225</v>
-      </c>
-      <c r="I13" t="s">
-        <v>64</v>
-      </c>
       <c r="J13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1655,7 +1655,7 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D14" t="s">
         <v>21</v>
@@ -1670,13 +1670,13 @@
         <v>19</v>
       </c>
       <c r="H14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I14" t="s">
-        <v>24</v>
+        <v>240</v>
       </c>
       <c r="J14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1687,10 +1687,10 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" t="s">
         <v>65</v>
-      </c>
-      <c r="D15" t="s">
-        <v>66</v>
       </c>
       <c r="E15" t="s">
         <v>17</v>
@@ -1702,13 +1702,13 @@
         <v>19</v>
       </c>
       <c r="H15" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J15" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1719,10 +1719,10 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" t="s">
         <v>25</v>
-      </c>
-      <c r="D16" t="s">
-        <v>26</v>
       </c>
       <c r="E16" t="s">
         <v>17</v>
@@ -1734,13 +1734,13 @@
         <v>19</v>
       </c>
       <c r="H16" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J16" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1751,28 +1751,28 @@
         <v>1</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>19</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1783,10 +1783,10 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E18" t="s">
         <v>17</v>
@@ -1798,13 +1798,13 @@
         <v>19</v>
       </c>
       <c r="H18" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J18" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1815,10 +1815,10 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" t="s">
         <v>34</v>
-      </c>
-      <c r="D19" t="s">
-        <v>35</v>
       </c>
       <c r="E19" t="s">
         <v>17</v>
@@ -1830,13 +1830,13 @@
         <v>19</v>
       </c>
       <c r="H19" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J19" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1847,7 +1847,7 @@
         <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D20" t="s">
         <v>16</v>
@@ -1862,13 +1862,13 @@
         <v>19</v>
       </c>
       <c r="H20" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J20" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1879,25 +1879,25 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" t="s">
         <v>68</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
+        <v>68</v>
+      </c>
+      <c r="F21" t="s">
         <v>69</v>
       </c>
-      <c r="E21" t="s">
-        <v>69</v>
-      </c>
-      <c r="F21" t="s">
+      <c r="H21" t="s">
+        <v>224</v>
+      </c>
+      <c r="I21" t="s">
         <v>70</v>
       </c>
-      <c r="H21" t="s">
-        <v>225</v>
-      </c>
-      <c r="I21" t="s">
-        <v>71</v>
-      </c>
       <c r="J21" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1908,25 +1908,25 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" t="s">
         <v>72</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
+        <v>72</v>
+      </c>
+      <c r="F22" t="s">
         <v>73</v>
       </c>
-      <c r="E22" t="s">
-        <v>73</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="H22" t="s">
+        <v>224</v>
+      </c>
+      <c r="I22" t="s">
         <v>74</v>
       </c>
-      <c r="H22" t="s">
-        <v>225</v>
-      </c>
-      <c r="I22" t="s">
-        <v>75</v>
-      </c>
       <c r="J22" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1937,26 +1937,26 @@
         <v>1</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>78</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1967,26 +1967,26 @@
         <v>1</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="E24" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1997,28 +1997,28 @@
         <v>1</v>
       </c>
       <c r="C25" t="s">
+        <v>81</v>
+      </c>
+      <c r="D25" t="s">
         <v>82</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>83</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>84</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>85</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
+        <v>224</v>
+      </c>
+      <c r="I25" t="s">
         <v>86</v>
       </c>
-      <c r="H25" t="s">
-        <v>225</v>
-      </c>
-      <c r="I25" t="s">
-        <v>87</v>
-      </c>
       <c r="J25" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -2029,25 +2029,25 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
+        <v>87</v>
+      </c>
+      <c r="D26" t="s">
         <v>88</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>89</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
+        <v>41</v>
+      </c>
+      <c r="H26" t="s">
+        <v>224</v>
+      </c>
+      <c r="I26" t="s">
         <v>90</v>
       </c>
-      <c r="F26" t="s">
-        <v>42</v>
-      </c>
-      <c r="H26" t="s">
-        <v>225</v>
-      </c>
-      <c r="I26" t="s">
-        <v>91</v>
-      </c>
       <c r="J26" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -2058,25 +2058,25 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
+        <v>91</v>
+      </c>
+      <c r="E27" t="s">
+        <v>83</v>
+      </c>
+      <c r="F27" t="s">
+        <v>84</v>
+      </c>
+      <c r="G27" t="s">
+        <v>85</v>
+      </c>
+      <c r="H27" t="s">
+        <v>224</v>
+      </c>
+      <c r="I27" t="s">
         <v>92</v>
       </c>
-      <c r="E27" t="s">
-        <v>84</v>
-      </c>
-      <c r="F27" t="s">
-        <v>85</v>
-      </c>
-      <c r="G27" t="s">
-        <v>86</v>
-      </c>
-      <c r="H27" t="s">
-        <v>225</v>
-      </c>
-      <c r="I27" t="s">
-        <v>93</v>
-      </c>
       <c r="J27" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -2087,28 +2087,28 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
+        <v>93</v>
+      </c>
+      <c r="D28" t="s">
+        <v>82</v>
+      </c>
+      <c r="E28" t="s">
         <v>94</v>
       </c>
-      <c r="D28" t="s">
-        <v>83</v>
-      </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
+        <v>30</v>
+      </c>
+      <c r="G28" t="s">
+        <v>85</v>
+      </c>
+      <c r="H28" t="s">
+        <v>224</v>
+      </c>
+      <c r="I28" t="s">
         <v>95</v>
       </c>
-      <c r="F28" t="s">
-        <v>31</v>
-      </c>
-      <c r="G28" t="s">
-        <v>86</v>
-      </c>
-      <c r="H28" t="s">
-        <v>225</v>
-      </c>
-      <c r="I28" t="s">
-        <v>96</v>
-      </c>
       <c r="J28" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -2119,25 +2119,25 @@
         <v>1</v>
       </c>
       <c r="C29" t="s">
+        <v>96</v>
+      </c>
+      <c r="D29" t="s">
         <v>97</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
+        <v>97</v>
+      </c>
+      <c r="F29" t="s">
         <v>98</v>
       </c>
-      <c r="E29" t="s">
-        <v>98</v>
-      </c>
-      <c r="F29" t="s">
+      <c r="H29" t="s">
+        <v>224</v>
+      </c>
+      <c r="I29" t="s">
         <v>99</v>
       </c>
-      <c r="H29" t="s">
-        <v>225</v>
-      </c>
-      <c r="I29" t="s">
-        <v>100</v>
-      </c>
       <c r="J29" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -2148,25 +2148,25 @@
         <v>1</v>
       </c>
       <c r="C30" t="s">
+        <v>100</v>
+      </c>
+      <c r="D30" t="s">
         <v>101</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F30" t="s">
+        <v>98</v>
+      </c>
+      <c r="H30" t="s">
+        <v>224</v>
+      </c>
+      <c r="I30" t="s">
         <v>102</v>
       </c>
-      <c r="E30" t="s">
-        <v>102</v>
-      </c>
-      <c r="F30" t="s">
-        <v>99</v>
-      </c>
-      <c r="H30" t="s">
-        <v>225</v>
-      </c>
-      <c r="I30" t="s">
-        <v>103</v>
-      </c>
       <c r="J30" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -2177,28 +2177,28 @@
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D31" t="s">
+        <v>132</v>
+      </c>
+      <c r="E31" t="s">
+        <v>120</v>
+      </c>
+      <c r="F31" t="s">
+        <v>121</v>
+      </c>
+      <c r="G31" t="s">
+        <v>107</v>
+      </c>
+      <c r="H31" t="s">
+        <v>224</v>
+      </c>
+      <c r="I31" t="s">
         <v>133</v>
       </c>
-      <c r="E31" t="s">
-        <v>121</v>
-      </c>
-      <c r="F31" t="s">
-        <v>122</v>
-      </c>
-      <c r="G31" t="s">
-        <v>108</v>
-      </c>
-      <c r="H31" t="s">
-        <v>225</v>
-      </c>
-      <c r="I31" t="s">
-        <v>134</v>
-      </c>
       <c r="J31" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -2209,28 +2209,28 @@
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D32">
         <v>200</v>
       </c>
       <c r="E32" t="s">
+        <v>120</v>
+      </c>
+      <c r="F32" t="s">
         <v>121</v>
       </c>
-      <c r="F32" t="s">
-        <v>122</v>
-      </c>
       <c r="G32" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H32" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I32" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J32" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -2241,28 +2241,28 @@
         <v>4</v>
       </c>
       <c r="C33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D33" t="s">
+        <v>136</v>
+      </c>
+      <c r="E33" t="s">
+        <v>120</v>
+      </c>
+      <c r="F33" t="s">
+        <v>121</v>
+      </c>
+      <c r="G33" t="s">
+        <v>107</v>
+      </c>
+      <c r="H33" t="s">
+        <v>224</v>
+      </c>
+      <c r="I33" t="s">
         <v>137</v>
       </c>
-      <c r="E33" t="s">
-        <v>121</v>
-      </c>
-      <c r="F33" t="s">
-        <v>122</v>
-      </c>
-      <c r="G33" t="s">
-        <v>108</v>
-      </c>
-      <c r="H33" t="s">
-        <v>225</v>
-      </c>
-      <c r="I33" t="s">
-        <v>138</v>
-      </c>
       <c r="J33" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -2273,28 +2273,28 @@
         <v>1</v>
       </c>
       <c r="C34" t="s">
+        <v>138</v>
+      </c>
+      <c r="D34" t="s">
         <v>139</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
+        <v>120</v>
+      </c>
+      <c r="F34" t="s">
+        <v>121</v>
+      </c>
+      <c r="G34" t="s">
+        <v>107</v>
+      </c>
+      <c r="H34" t="s">
+        <v>224</v>
+      </c>
+      <c r="I34" t="s">
         <v>140</v>
       </c>
-      <c r="E34" t="s">
-        <v>121</v>
-      </c>
-      <c r="F34" t="s">
-        <v>122</v>
-      </c>
-      <c r="G34" t="s">
-        <v>108</v>
-      </c>
-      <c r="H34" t="s">
-        <v>225</v>
-      </c>
-      <c r="I34" t="s">
-        <v>141</v>
-      </c>
       <c r="J34" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -2305,28 +2305,28 @@
         <v>1</v>
       </c>
       <c r="C35" t="s">
+        <v>141</v>
+      </c>
+      <c r="D35" t="s">
         <v>142</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
+        <v>120</v>
+      </c>
+      <c r="F35" t="s">
+        <v>121</v>
+      </c>
+      <c r="G35" t="s">
+        <v>107</v>
+      </c>
+      <c r="H35" t="s">
+        <v>224</v>
+      </c>
+      <c r="I35" t="s">
         <v>143</v>
       </c>
-      <c r="E35" t="s">
-        <v>121</v>
-      </c>
-      <c r="F35" t="s">
-        <v>122</v>
-      </c>
-      <c r="G35" t="s">
-        <v>108</v>
-      </c>
-      <c r="H35" t="s">
-        <v>225</v>
-      </c>
-      <c r="I35" t="s">
-        <v>144</v>
-      </c>
       <c r="J35" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -2337,28 +2337,28 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
+        <v>144</v>
+      </c>
+      <c r="D36" t="s">
         <v>145</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
+        <v>120</v>
+      </c>
+      <c r="F36" t="s">
+        <v>121</v>
+      </c>
+      <c r="G36" t="s">
+        <v>107</v>
+      </c>
+      <c r="H36" t="s">
+        <v>224</v>
+      </c>
+      <c r="I36" t="s">
         <v>146</v>
       </c>
-      <c r="E36" t="s">
-        <v>121</v>
-      </c>
-      <c r="F36" t="s">
-        <v>122</v>
-      </c>
-      <c r="G36" t="s">
-        <v>108</v>
-      </c>
-      <c r="H36" t="s">
-        <v>225</v>
-      </c>
-      <c r="I36" t="s">
-        <v>147</v>
-      </c>
       <c r="J36" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -2369,28 +2369,28 @@
         <v>1</v>
       </c>
       <c r="C37" t="s">
+        <v>147</v>
+      </c>
+      <c r="D37" t="s">
         <v>148</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
+        <v>120</v>
+      </c>
+      <c r="F37" t="s">
+        <v>121</v>
+      </c>
+      <c r="G37" t="s">
+        <v>107</v>
+      </c>
+      <c r="H37" t="s">
+        <v>224</v>
+      </c>
+      <c r="I37" t="s">
         <v>149</v>
       </c>
-      <c r="E37" t="s">
-        <v>121</v>
-      </c>
-      <c r="F37" t="s">
-        <v>122</v>
-      </c>
-      <c r="G37" t="s">
-        <v>108</v>
-      </c>
-      <c r="H37" t="s">
-        <v>225</v>
-      </c>
-      <c r="I37" t="s">
-        <v>150</v>
-      </c>
       <c r="J37" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -2401,28 +2401,28 @@
         <v>1</v>
       </c>
       <c r="C38" t="s">
+        <v>103</v>
+      </c>
+      <c r="D38" t="s">
         <v>104</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>105</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F38" t="s">
         <v>106</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G38" t="s">
         <v>107</v>
       </c>
-      <c r="G38" t="s">
+      <c r="H38" t="s">
+        <v>224</v>
+      </c>
+      <c r="I38" t="s">
         <v>108</v>
       </c>
-      <c r="H38" t="s">
-        <v>225</v>
-      </c>
-      <c r="I38" t="s">
-        <v>109</v>
-      </c>
       <c r="J38" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -2433,28 +2433,28 @@
         <v>1</v>
       </c>
       <c r="C39" t="s">
+        <v>150</v>
+      </c>
+      <c r="D39" t="s">
         <v>151</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>152</v>
       </c>
-      <c r="E39" t="s">
+      <c r="F39" t="s">
         <v>153</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
+        <v>107</v>
+      </c>
+      <c r="H39" t="s">
+        <v>224</v>
+      </c>
+      <c r="I39" t="s">
         <v>154</v>
       </c>
-      <c r="G39" t="s">
-        <v>108</v>
-      </c>
-      <c r="H39" t="s">
-        <v>225</v>
-      </c>
-      <c r="I39" t="s">
-        <v>155</v>
-      </c>
       <c r="J39" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -2465,28 +2465,28 @@
         <v>1</v>
       </c>
       <c r="C40" t="s">
+        <v>109</v>
+      </c>
+      <c r="D40" t="s">
         <v>110</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>111</v>
       </c>
-      <c r="E40" t="s">
+      <c r="F40" t="s">
         <v>112</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G40" t="s">
+        <v>107</v>
+      </c>
+      <c r="H40" t="s">
+        <v>224</v>
+      </c>
+      <c r="I40" t="s">
         <v>113</v>
       </c>
-      <c r="G40" t="s">
-        <v>108</v>
-      </c>
-      <c r="H40" t="s">
-        <v>225</v>
-      </c>
-      <c r="I40" t="s">
-        <v>114</v>
-      </c>
       <c r="J40" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -2497,28 +2497,28 @@
         <v>1</v>
       </c>
       <c r="C41" t="s">
+        <v>155</v>
+      </c>
+      <c r="D41" t="s">
         <v>156</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
+        <v>120</v>
+      </c>
+      <c r="F41" t="s">
+        <v>121</v>
+      </c>
+      <c r="G41" t="s">
+        <v>107</v>
+      </c>
+      <c r="H41" t="s">
+        <v>224</v>
+      </c>
+      <c r="I41" t="s">
         <v>157</v>
       </c>
-      <c r="E41" t="s">
-        <v>121</v>
-      </c>
-      <c r="F41" t="s">
-        <v>122</v>
-      </c>
-      <c r="G41" t="s">
-        <v>108</v>
-      </c>
-      <c r="H41" t="s">
-        <v>225</v>
-      </c>
-      <c r="I41" t="s">
-        <v>158</v>
-      </c>
       <c r="J41" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -2529,28 +2529,28 @@
         <v>1</v>
       </c>
       <c r="C42" t="s">
+        <v>158</v>
+      </c>
+      <c r="D42" t="s">
         <v>159</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
+        <v>120</v>
+      </c>
+      <c r="F42" t="s">
+        <v>121</v>
+      </c>
+      <c r="G42" t="s">
+        <v>107</v>
+      </c>
+      <c r="H42" t="s">
+        <v>224</v>
+      </c>
+      <c r="I42" t="s">
         <v>160</v>
       </c>
-      <c r="E42" t="s">
-        <v>121</v>
-      </c>
-      <c r="F42" t="s">
-        <v>122</v>
-      </c>
-      <c r="G42" t="s">
-        <v>108</v>
-      </c>
-      <c r="H42" t="s">
-        <v>225</v>
-      </c>
-      <c r="I42" t="s">
-        <v>161</v>
-      </c>
       <c r="J42" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -2561,28 +2561,28 @@
         <v>1</v>
       </c>
       <c r="C43" t="s">
+        <v>161</v>
+      </c>
+      <c r="D43" t="s">
         <v>162</v>
       </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
+        <v>120</v>
+      </c>
+      <c r="F43" t="s">
+        <v>121</v>
+      </c>
+      <c r="G43" t="s">
+        <v>107</v>
+      </c>
+      <c r="H43" t="s">
+        <v>224</v>
+      </c>
+      <c r="I43" t="s">
         <v>163</v>
       </c>
-      <c r="E43" t="s">
-        <v>121</v>
-      </c>
-      <c r="F43" t="s">
-        <v>122</v>
-      </c>
-      <c r="G43" t="s">
-        <v>108</v>
-      </c>
-      <c r="H43" t="s">
-        <v>225</v>
-      </c>
-      <c r="I43" t="s">
-        <v>164</v>
-      </c>
       <c r="J43" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -2593,28 +2593,28 @@
         <v>1</v>
       </c>
       <c r="C44" t="s">
+        <v>164</v>
+      </c>
+      <c r="D44" t="s">
         <v>165</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
+        <v>120</v>
+      </c>
+      <c r="F44" t="s">
+        <v>121</v>
+      </c>
+      <c r="G44" t="s">
+        <v>107</v>
+      </c>
+      <c r="H44" t="s">
+        <v>224</v>
+      </c>
+      <c r="I44" t="s">
         <v>166</v>
       </c>
-      <c r="E44" t="s">
-        <v>121</v>
-      </c>
-      <c r="F44" t="s">
-        <v>122</v>
-      </c>
-      <c r="G44" t="s">
-        <v>108</v>
-      </c>
-      <c r="H44" t="s">
-        <v>225</v>
-      </c>
-      <c r="I44" t="s">
-        <v>167</v>
-      </c>
       <c r="J44" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -2625,28 +2625,28 @@
         <v>1</v>
       </c>
       <c r="C45" t="s">
+        <v>114</v>
+      </c>
+      <c r="D45" t="s">
         <v>115</v>
       </c>
-      <c r="D45" t="s">
+      <c r="E45" t="s">
         <v>116</v>
       </c>
-      <c r="E45" t="s">
+      <c r="F45" t="s">
         <v>117</v>
       </c>
-      <c r="F45" t="s">
+      <c r="G45" t="s">
         <v>118</v>
       </c>
-      <c r="G45" t="s">
+      <c r="H45" t="s">
+        <v>224</v>
+      </c>
+      <c r="I45" t="s">
         <v>119</v>
       </c>
-      <c r="H45" t="s">
-        <v>225</v>
-      </c>
-      <c r="I45" t="s">
-        <v>120</v>
-      </c>
       <c r="J45" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -2657,28 +2657,28 @@
         <v>3</v>
       </c>
       <c r="C46" t="s">
+        <v>218</v>
+      </c>
+      <c r="D46" t="s">
         <v>219</v>
       </c>
-      <c r="D46" t="s">
-        <v>220</v>
-      </c>
       <c r="E46" t="s">
+        <v>120</v>
+      </c>
+      <c r="F46" t="s">
         <v>121</v>
       </c>
-      <c r="F46" t="s">
+      <c r="G46" t="s">
+        <v>107</v>
+      </c>
+      <c r="H46" t="s">
+        <v>224</v>
+      </c>
+      <c r="I46" t="s">
         <v>122</v>
       </c>
-      <c r="G46" t="s">
-        <v>108</v>
-      </c>
-      <c r="H46" t="s">
-        <v>225</v>
-      </c>
-      <c r="I46" t="s">
-        <v>123</v>
-      </c>
       <c r="J46" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -2689,28 +2689,28 @@
         <v>1</v>
       </c>
       <c r="C47" t="s">
+        <v>123</v>
+      </c>
+      <c r="D47" t="s">
         <v>124</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
+        <v>120</v>
+      </c>
+      <c r="F47" t="s">
+        <v>121</v>
+      </c>
+      <c r="G47" t="s">
+        <v>107</v>
+      </c>
+      <c r="H47" t="s">
+        <v>224</v>
+      </c>
+      <c r="I47" t="s">
         <v>125</v>
       </c>
-      <c r="E47" t="s">
-        <v>121</v>
-      </c>
-      <c r="F47" t="s">
-        <v>122</v>
-      </c>
-      <c r="G47" t="s">
-        <v>108</v>
-      </c>
-      <c r="H47" t="s">
-        <v>225</v>
-      </c>
-      <c r="I47" t="s">
-        <v>126</v>
-      </c>
       <c r="J47" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -2721,28 +2721,28 @@
         <v>1</v>
       </c>
       <c r="C48" t="s">
+        <v>126</v>
+      </c>
+      <c r="D48" t="s">
         <v>127</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
+        <v>105</v>
+      </c>
+      <c r="F48" t="s">
+        <v>106</v>
+      </c>
+      <c r="G48" t="s">
+        <v>107</v>
+      </c>
+      <c r="H48" t="s">
+        <v>224</v>
+      </c>
+      <c r="I48" t="s">
         <v>128</v>
       </c>
-      <c r="E48" t="s">
-        <v>106</v>
-      </c>
-      <c r="F48" t="s">
-        <v>107</v>
-      </c>
-      <c r="G48" t="s">
-        <v>108</v>
-      </c>
-      <c r="H48" t="s">
-        <v>225</v>
-      </c>
-      <c r="I48" t="s">
-        <v>129</v>
-      </c>
       <c r="J48" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -2753,28 +2753,28 @@
         <v>1</v>
       </c>
       <c r="C49" t="s">
+        <v>129</v>
+      </c>
+      <c r="D49" t="s">
         <v>130</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
+        <v>120</v>
+      </c>
+      <c r="F49" t="s">
+        <v>121</v>
+      </c>
+      <c r="G49" t="s">
+        <v>107</v>
+      </c>
+      <c r="H49" t="s">
+        <v>224</v>
+      </c>
+      <c r="I49" t="s">
         <v>131</v>
       </c>
-      <c r="E49" t="s">
-        <v>121</v>
-      </c>
-      <c r="F49" t="s">
-        <v>122</v>
-      </c>
-      <c r="G49" t="s">
-        <v>108</v>
-      </c>
-      <c r="H49" t="s">
-        <v>225</v>
-      </c>
-      <c r="I49" t="s">
-        <v>132</v>
-      </c>
       <c r="J49" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -2785,28 +2785,28 @@
         <v>1</v>
       </c>
       <c r="C50" t="s">
+        <v>167</v>
+      </c>
+      <c r="D50" t="s">
         <v>168</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
+        <v>120</v>
+      </c>
+      <c r="F50" t="s">
+        <v>121</v>
+      </c>
+      <c r="G50" t="s">
+        <v>107</v>
+      </c>
+      <c r="H50" t="s">
+        <v>224</v>
+      </c>
+      <c r="I50" t="s">
         <v>169</v>
       </c>
-      <c r="E50" t="s">
-        <v>121</v>
-      </c>
-      <c r="F50" t="s">
-        <v>122</v>
-      </c>
-      <c r="G50" t="s">
-        <v>108</v>
-      </c>
-      <c r="H50" t="s">
-        <v>225</v>
-      </c>
-      <c r="I50" t="s">
-        <v>170</v>
-      </c>
       <c r="J50" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -2817,28 +2817,28 @@
         <v>2</v>
       </c>
       <c r="C51" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D51" t="s">
+        <v>170</v>
+      </c>
+      <c r="E51" t="s">
+        <v>120</v>
+      </c>
+      <c r="F51" t="s">
+        <v>121</v>
+      </c>
+      <c r="G51" t="s">
+        <v>107</v>
+      </c>
+      <c r="H51" t="s">
+        <v>224</v>
+      </c>
+      <c r="I51" t="s">
         <v>171</v>
       </c>
-      <c r="E51" t="s">
-        <v>121</v>
-      </c>
-      <c r="F51" t="s">
-        <v>122</v>
-      </c>
-      <c r="G51" t="s">
-        <v>108</v>
-      </c>
-      <c r="H51" t="s">
-        <v>225</v>
-      </c>
-      <c r="I51" t="s">
-        <v>172</v>
-      </c>
       <c r="J51" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -2849,26 +2849,26 @@
         <v>1</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F52" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="F52" s="1" t="s">
+      <c r="G52" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="G52" s="1" t="s">
+      <c r="H52" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="I52" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="H52" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="I52" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="J52" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -2879,25 +2879,25 @@
         <v>1</v>
       </c>
       <c r="C53" t="s">
+        <v>177</v>
+      </c>
+      <c r="D53" t="s">
         <v>178</v>
       </c>
-      <c r="D53" t="s">
+      <c r="E53" t="s">
+        <v>178</v>
+      </c>
+      <c r="F53" t="s">
         <v>179</v>
       </c>
-      <c r="E53" t="s">
-        <v>179</v>
-      </c>
-      <c r="F53" t="s">
+      <c r="H53" t="s">
+        <v>224</v>
+      </c>
+      <c r="I53" t="s">
         <v>180</v>
       </c>
-      <c r="H53" t="s">
-        <v>225</v>
-      </c>
-      <c r="I53" t="s">
-        <v>181</v>
-      </c>
       <c r="J53" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -2908,25 +2908,25 @@
         <v>1</v>
       </c>
       <c r="C54" t="s">
+        <v>181</v>
+      </c>
+      <c r="D54" t="s">
+        <v>230</v>
+      </c>
+      <c r="E54" t="s">
+        <v>230</v>
+      </c>
+      <c r="F54" t="s">
         <v>182</v>
       </c>
-      <c r="D54" t="s">
-        <v>231</v>
-      </c>
-      <c r="E54" t="s">
-        <v>231</v>
-      </c>
-      <c r="F54" t="s">
+      <c r="H54" t="s">
+        <v>224</v>
+      </c>
+      <c r="I54" t="s">
         <v>183</v>
       </c>
-      <c r="H54" t="s">
-        <v>225</v>
-      </c>
-      <c r="I54" t="s">
-        <v>184</v>
-      </c>
       <c r="J54" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -2937,25 +2937,25 @@
         <v>1</v>
       </c>
       <c r="C55" t="s">
+        <v>184</v>
+      </c>
+      <c r="D55" t="s">
         <v>185</v>
       </c>
-      <c r="D55" t="s">
+      <c r="E55" t="s">
+        <v>185</v>
+      </c>
+      <c r="F55" t="s">
         <v>186</v>
       </c>
-      <c r="E55" t="s">
-        <v>186</v>
-      </c>
-      <c r="F55" t="s">
+      <c r="H55" t="s">
+        <v>224</v>
+      </c>
+      <c r="I55" t="s">
         <v>187</v>
       </c>
-      <c r="H55" t="s">
-        <v>225</v>
-      </c>
-      <c r="I55" t="s">
-        <v>188</v>
-      </c>
       <c r="J55" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -2966,28 +2966,28 @@
         <v>1</v>
       </c>
       <c r="C56" t="s">
+        <v>188</v>
+      </c>
+      <c r="D56" t="s">
         <v>189</v>
       </c>
-      <c r="D56" t="s">
+      <c r="E56" t="s">
+        <v>189</v>
+      </c>
+      <c r="F56" t="s">
         <v>190</v>
       </c>
-      <c r="E56" t="s">
-        <v>190</v>
-      </c>
-      <c r="F56" t="s">
+      <c r="G56" t="s">
         <v>191</v>
       </c>
-      <c r="G56" t="s">
+      <c r="H56" t="s">
+        <v>224</v>
+      </c>
+      <c r="I56" t="s">
         <v>192</v>
       </c>
-      <c r="H56" t="s">
-        <v>225</v>
-      </c>
-      <c r="I56" t="s">
-        <v>193</v>
-      </c>
       <c r="J56" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -2998,25 +2998,25 @@
         <v>1</v>
       </c>
       <c r="C57" t="s">
+        <v>193</v>
+      </c>
+      <c r="D57" t="s">
         <v>194</v>
       </c>
-      <c r="D57" t="s">
+      <c r="E57" t="s">
+        <v>194</v>
+      </c>
+      <c r="F57" t="s">
+        <v>182</v>
+      </c>
+      <c r="H57" t="s">
+        <v>224</v>
+      </c>
+      <c r="I57" t="s">
         <v>195</v>
       </c>
-      <c r="E57" t="s">
-        <v>195</v>
-      </c>
-      <c r="F57" t="s">
-        <v>183</v>
-      </c>
-      <c r="H57" t="s">
-        <v>225</v>
-      </c>
-      <c r="I57" t="s">
-        <v>196</v>
-      </c>
       <c r="J57" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -3027,25 +3027,25 @@
         <v>1</v>
       </c>
       <c r="C58" t="s">
+        <v>196</v>
+      </c>
+      <c r="D58" t="s">
         <v>197</v>
       </c>
-      <c r="D58" t="s">
+      <c r="E58" t="s">
+        <v>197</v>
+      </c>
+      <c r="F58" t="s">
         <v>198</v>
       </c>
-      <c r="E58" t="s">
-        <v>198</v>
-      </c>
-      <c r="F58" t="s">
+      <c r="H58" t="s">
+        <v>224</v>
+      </c>
+      <c r="I58" t="s">
         <v>199</v>
       </c>
-      <c r="H58" t="s">
-        <v>225</v>
-      </c>
-      <c r="I58" t="s">
-        <v>200</v>
-      </c>
       <c r="J58" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="59" spans="1:10">
@@ -3056,28 +3056,28 @@
         <v>1</v>
       </c>
       <c r="C59" t="s">
+        <v>200</v>
+      </c>
+      <c r="D59" t="s">
         <v>201</v>
       </c>
-      <c r="D59" t="s">
+      <c r="E59" t="s">
         <v>202</v>
       </c>
-      <c r="E59" t="s">
+      <c r="F59" t="s">
+        <v>202</v>
+      </c>
+      <c r="G59" t="s">
         <v>203</v>
       </c>
-      <c r="F59" t="s">
-        <v>203</v>
-      </c>
-      <c r="G59" t="s">
+      <c r="H59" t="s">
+        <v>224</v>
+      </c>
+      <c r="I59" t="s">
         <v>204</v>
       </c>
-      <c r="H59" t="s">
-        <v>225</v>
-      </c>
-      <c r="I59" t="s">
-        <v>205</v>
-      </c>
       <c r="J59" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="60" spans="1:10">
@@ -3088,25 +3088,25 @@
         <v>1</v>
       </c>
       <c r="C60" t="s">
+        <v>205</v>
+      </c>
+      <c r="D60" t="s">
         <v>206</v>
       </c>
-      <c r="D60" t="s">
+      <c r="E60" t="s">
         <v>207</v>
-      </c>
-      <c r="E60" t="s">
-        <v>208</v>
       </c>
       <c r="F60">
         <v>805</v>
       </c>
       <c r="H60" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I60" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="J60" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="61" spans="1:10">
@@ -3117,36 +3117,36 @@
         <v>1</v>
       </c>
       <c r="C61" t="s">
+        <v>209</v>
+      </c>
+      <c r="D61" t="s">
         <v>210</v>
       </c>
-      <c r="D61" t="s">
-        <v>211</v>
-      </c>
       <c r="E61" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F61" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H61" t="s">
+        <v>238</v>
+      </c>
+      <c r="I61" t="s">
         <v>239</v>
       </c>
-      <c r="I61" t="s">
-        <v>240</v>
-      </c>
       <c r="J61" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="65" spans="8:9">
       <c r="H65" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I65" s="7"/>
     </row>
     <row r="66" spans="8:9">
       <c r="H66" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="I66" s="3">
         <v>56</v>
@@ -3154,7 +3154,7 @@
     </row>
     <row r="67" spans="8:9">
       <c r="H67" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I67" s="3">
         <v>69</v>
@@ -3162,7 +3162,7 @@
     </row>
     <row r="68" spans="8:9">
       <c r="H68" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I68" s="3">
         <v>0</v>
@@ -3170,7 +3170,7 @@
     </row>
     <row r="69" spans="8:9">
       <c r="H69" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I69" s="3">
         <v>3</v>
@@ -3178,7 +3178,7 @@
     </row>
     <row r="70" spans="8:9">
       <c r="H70" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I70" s="5">
         <v>1</v>

</xml_diff>